<commit_message>
Fix: Markdown counter 0-based indexing and auto new thread on no code block
- Fix markdown counter to fetch BEFORE increment (starts at 0, not 1)
- Set counter to 1 after initial prompt to skip markdown-content-0
- Auto create new thread when AI response has no code block
- Add emergency and scheduled new thread with initial prompt
- Add test mode (5 rows/thread) with UI checkbox
- Track rowsInCurrentThread separately from processedRows
- Only reset rowsInCurrentThread after createNewThread(), not markdownCounter
- Add comprehensive documentation for markdown counter logic
</commit_message>
<xml_diff>
--- a/src/IngredientName/Food Exclusion Tag_RootFile_Part1.xlsx
+++ b/src/IngredientName/Food Exclusion Tag_RootFile_Part1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="1092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2533" uniqueCount="1092">
   <si>
     <t>_id</t>
   </si>
@@ -5554,11 +5554,11 @@
         <v>181</v>
       </c>
       <c r="E68" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Dairy, Sweeteners")</f>
-        <v>Dairy, Sweeteners</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>21</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Beef, Sweeteners")</f>
+        <v>Beef, Sweeteners</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
@@ -5583,10 +5583,12 @@
         <v>183</v>
       </c>
       <c r="E69" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sweeteners")</f>
-        <v>Sweeteners</v>
-      </c>
-      <c r="F69" s="6"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Beef, Sweeteners")</f>
+        <v>Beef, Sweeteners</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
@@ -5610,11 +5612,11 @@
         <v>185</v>
       </c>
       <c r="E70" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Dairy, Sweeteners")</f>
-        <v>Dairy, Sweeteners</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>21</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Beef, Sweeteners")</f>
+        <v>Beef, Sweeteners</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
@@ -5639,11 +5641,11 @@
         <v>187</v>
       </c>
       <c r="E71" s="6" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Dairy, Sweeteners")</f>
-        <v>Dairy, Sweeteners</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>21</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Beef, Sweeteners")</f>
+        <v>Beef, Sweeteners</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
@@ -10872,7 +10874,7 @@
         <v>534</v>
       </c>
       <c r="C250" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D250" s="6" t="s">
         <v>572</v>
@@ -10903,7 +10905,7 @@
       </c>
       <c r="B251" s="4"/>
       <c r="C251" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D251" s="6" t="s">
         <v>574</v>
@@ -10961,7 +10963,7 @@
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D253" s="6" t="s">
         <v>578</v>

</xml_diff>